<commit_message>
Fill in the Japanese Kanji form
</commit_message>
<xml_diff>
--- a/讀音表.xlsx
+++ b/讀音表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10760\Desktop\日語拓展\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyanidin/Documents/HKBU/Github/Noroki/Rime/rime-jyutping-extension/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D807ADA4-5C43-41A0-AC31-CF0760D58988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A96A0C-1701-1647-9FB3-DE165B712750}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="540" windowWidth="14730" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="219">
   <si>
     <t>匂</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>shibo-ru</t>
-  </si>
-  <si>
-    <t>saku</t>
   </si>
   <si>
     <t>zhà / ㄓㄚˋ</t>
@@ -347,7 +344,7 @@
         <u/>
         <sz val="11"/>
         <color theme="10"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -370,7 +367,7 @@
         <u/>
         <sz val="11"/>
         <color theme="10"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -408,7 +405,7 @@
         <u/>
         <sz val="11"/>
         <color theme="10"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -446,7 +443,7 @@
         <u/>
         <sz val="11"/>
         <color theme="10"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -487,7 +484,7 @@
         <u/>
         <sz val="11"/>
         <color theme="10"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -630,16 +627,199 @@
     <t>喰</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>暫擬讀音</t>
+  </si>
+  <si>
+    <t>dam2</t>
+  </si>
+  <si>
+    <t>sap6</t>
+  </si>
+  <si>
+    <t>jap6</t>
+  </si>
+  <si>
+    <t>gan1</t>
+  </si>
+  <si>
+    <t>san1</t>
+  </si>
+  <si>
+    <t>saan1</t>
+  </si>
+  <si>
+    <t>kaa1</t>
+  </si>
+  <si>
+    <t>fat6</t>
+  </si>
+  <si>
+    <t>maai6</t>
+  </si>
+  <si>
+    <t>gaa2</t>
+  </si>
+  <si>
+    <t>jik6</t>
+  </si>
+  <si>
+    <t>zaak6</t>
+  </si>
+  <si>
+    <t>ban1</t>
+  </si>
+  <si>
+    <t>bin1</t>
+  </si>
+  <si>
+    <t>gip3</t>
+  </si>
+  <si>
+    <t>ngai6</t>
+  </si>
+  <si>
+    <t>siu3</t>
+  </si>
+  <si>
+    <t>tung1</t>
+  </si>
+  <si>
+    <t>kwai1</t>
+  </si>
+  <si>
+    <t>cyun4</t>
+  </si>
+  <si>
+    <t>bin6</t>
+  </si>
+  <si>
+    <t>jing3</t>
+  </si>
+  <si>
+    <t>hip3</t>
+  </si>
+  <si>
+    <t>cung1</t>
+  </si>
+  <si>
+    <t>ceon1</t>
+  </si>
+  <si>
+    <t>mui4</t>
+  </si>
+  <si>
+    <t>wan4</t>
+  </si>
+  <si>
+    <t>zeot1</t>
+  </si>
+  <si>
+    <t>tin4</t>
+  </si>
+  <si>
+    <t>lai6</t>
+  </si>
+  <si>
+    <t>jan6</t>
+  </si>
+  <si>
+    <t>sai3</t>
+  </si>
+  <si>
+    <t>ping4</t>
+  </si>
+  <si>
+    <t>coeng1</t>
+  </si>
+  <si>
+    <t>lou5</t>
+  </si>
+  <si>
+    <t>sik6</t>
+  </si>
+  <si>
+    <t>zaa3</t>
+  </si>
+  <si>
+    <t>san4</t>
+  </si>
+  <si>
+    <t>dung6</t>
+  </si>
+  <si>
+    <t>faa1</t>
+  </si>
+  <si>
+    <t>bing2</t>
+  </si>
+  <si>
+    <t>zan1</t>
+  </si>
+  <si>
+    <t>gin1</t>
+  </si>
+  <si>
+    <t>leong4</t>
+  </si>
+  <si>
+    <t>mo4</t>
+  </si>
+  <si>
+    <t>jat1</t>
+  </si>
+  <si>
+    <t>zi2</t>
+  </si>
+  <si>
+    <t>muk6</t>
+  </si>
+  <si>
+    <t>mung6</t>
+  </si>
+  <si>
+    <t>mei5</t>
+  </si>
+  <si>
+    <t>辯</t>
+  </si>
+  <si>
+    <t>瓣</t>
+  </si>
+  <si>
+    <t>辨</t>
+  </si>
+  <si>
+    <t>faan2</t>
+  </si>
+  <si>
+    <t>意思</t>
+  </si>
+  <si>
+    <t>古代一种尊贵的冠</t>
+  </si>
+  <si>
+    <t>同「榨」</t>
+  </si>
+  <si>
+    <t>saku(慣)</t>
+  </si>
+  <si>
+    <t>haa6</t>
+  </si>
+  <si>
+    <t>jyu5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -666,7 +846,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -674,14 +854,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -706,8 +886,14 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -726,8 +912,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -813,12 +1005,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA2A9B1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -842,6 +1043,21 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -857,10 +1073,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1138,24 +1369,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28:B29"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="34.1640625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="11"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="B1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="31" thickBot="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1168,8 +1411,11 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="31" thickBot="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1182,8 +1428,11 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1196,8 +1445,11 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16" thickBot="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1210,8 +1462,11 @@
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="31" thickBot="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1224,8 +1479,11 @@
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31" thickBot="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1238,8 +1496,11 @@
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31" thickBot="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1252,30 +1513,37 @@
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14">
+      <c r="G8" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="19">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" thickBot="1">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="20"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="16" thickBot="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1288,8 +1556,11 @@
       <c r="D11" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="31" thickBot="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1302,8 +1573,11 @@
       <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31" thickBot="1">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1316,8 +1590,11 @@
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1330,8 +1607,11 @@
       <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31" thickBot="1">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1344,30 +1624,37 @@
       <c r="D15" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="14">
+      <c r="G15" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="19">
         <v>14</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
+      <c r="G16" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16" thickBot="1">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="20"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="1:7" ht="31" thickBot="1">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1380,8 +1667,11 @@
       <c r="D18" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1394,8 +1684,11 @@
       <c r="D19" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="31" thickBot="1">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1408,8 +1701,11 @@
       <c r="D20" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="31" thickBot="1">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1422,8 +1718,11 @@
       <c r="D21" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16" thickBot="1">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1437,7 +1736,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="31" thickBot="1">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1450,8 +1749,11 @@
       <c r="D23" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="31" thickBot="1">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1464,435 +1766,588 @@
       <c r="D24" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="14">
+      <c r="G24" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16" customHeight="1">
+      <c r="A25" s="19">
         <v>22</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="19" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
+      <c r="D25" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16" thickBot="1">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="15"/>
-    </row>
-    <row r="27" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" spans="1:7" ht="31" thickBot="1">
       <c r="A27" s="1">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="G27" s="11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30">
+      <c r="A28" s="19">
+        <v>24</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="14">
-        <v>24</v>
-      </c>
-      <c r="B28" s="14" t="s">
+      <c r="C28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="16" thickBot="1">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="15"/>
-    </row>
-    <row r="30" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="20"/>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7" ht="31" thickBot="1">
       <c r="A30" s="1">
         <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="31" thickBot="1">
       <c r="A31" s="1">
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="31" thickBot="1">
       <c r="A32" s="1">
         <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="31" thickBot="1">
       <c r="A33" s="1">
         <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="31" thickBot="1">
       <c r="A34" s="1">
         <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="31" thickBot="1">
       <c r="A35" s="1">
         <v>30</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="31" thickBot="1">
       <c r="A36" s="1">
         <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="31" thickBot="1">
       <c r="A37" s="1">
         <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="G37" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16" thickBot="1"/>
+    <row r="39" spans="1:7" ht="46" thickBot="1">
+      <c r="B39" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="D39" s="18"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="13"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="4" t="s">
+      <c r="G39" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="16" thickBot="1">
+      <c r="B40" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="D40" s="18"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="81" thickBot="1">
+      <c r="B41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="17"/>
+      <c r="E41" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="G41" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="193" thickBot="1">
+      <c r="B42" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="157.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="D42" s="18"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="5" t="s">
+      <c r="G42" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="46" thickBot="1">
+      <c r="B43" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="17"/>
+      <c r="E43" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="65" thickBot="1">
+      <c r="B44" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D44" s="17"/>
+      <c r="E44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="G44" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="106" thickBot="1">
+      <c r="B45" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="17"/>
+      <c r="E45" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="G45" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="129" thickBot="1">
+      <c r="B46" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="114.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="D46" s="17"/>
+      <c r="E46" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="G46" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="61" thickBot="1">
+      <c r="B47" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="D47" s="17"/>
+      <c r="E47" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="G47" s="13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="193" thickBot="1">
+      <c r="B48" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="157.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F48" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="302.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G48" s="25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="330" thickBot="1">
       <c r="A49" s="8"/>
       <c r="B49" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="17"/>
+      <c r="E49" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G49" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F49" s="4" t="s">
+    </row>
+    <row r="51" spans="1:7">
+      <c r="B51" t="s">
         <v>135</v>
       </c>
-      <c r="G49" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+      <c r="G51" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="B52" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+      <c r="G52" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="B53" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+      <c r="G53" s="14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="B54" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+      <c r="G54" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="B55" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+      <c r="G55" s="14" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="B56" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="8"/>
       <c r="B57" t="s">
+        <v>141</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="B58" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B58" s="6" t="s">
+      <c r="G58" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="B59" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B59" s="6" t="s">
+      <c r="G59" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="B61" s="7" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B61" s="7" t="s">
+      <c r="G61" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="B62" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G62" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="8"/>
       <c r="B63" s="9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="B64" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="B65" s="7" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B65" s="7" t="s">
+      <c r="C65" t="s">
+        <v>209</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="B66" s="7"/>
+      <c r="C66" t="s">
+        <v>210</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="B67" s="7"/>
+      <c r="C67" t="s">
+        <v>211</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="51">
+      <c r="B68" s="7"/>
+      <c r="C68" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F68" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="B69" s="7" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B66" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="8"/>
-      <c r="B67" t="s">
-        <v>158</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="G69" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="8"/>
+      <c r="B70" t="s">
+        <v>157</v>
+      </c>
+      <c r="C70" t="s">
+        <v>152</v>
+      </c>
+      <c r="D70" t="s">
+        <v>150</v>
+      </c>
+      <c r="E70" t="s">
         <v>153</v>
       </c>
-      <c r="D67" t="s">
-        <v>151</v>
-      </c>
-      <c r="E67" t="s">
-        <v>154</v>
+      <c r="G70" s="11" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="27">
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="D9:D10"/>
@@ -1905,7 +2360,6 @@
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C49:D49"/>
@@ -1915,6 +2369,12 @@
     <mergeCell ref="C42:E42"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C44:D44"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F25:F26"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>